<commit_message>
Update QS doc example
</commit_message>
<xml_diff>
--- a/client/examples/buildingScenario.xlsx
+++ b/client/examples/buildingScenario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepos\digital-twins-samples\AdtSampleApp\SampleClientApp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\baanders\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC4DB0C-29D8-4610-8519-05CF97474F88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93A7538-C8B2-4710-9307-B44B66FECA21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4035" yWindow="1500" windowWidth="16875" windowHeight="12900" xr2:uid="{B6154E4F-774F-4730-84F3-5195ADBCD94E}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{B6154E4F-774F-4730-84F3-5195ADBCD94E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>ModelID</t>
   </si>
@@ -75,6 +75,15 @@
   </si>
   <si>
     <t>Room0</t>
+  </si>
+  <si>
+    <t>BuildingA</t>
+  </si>
+  <si>
+    <t>{"Date": 2001}</t>
+  </si>
+  <si>
+    <t>dtmi:example:Building;1</t>
   </si>
 </sst>
 </file>
@@ -432,15 +441,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2E4B3A2-EF53-41B2-9F0F-6F5502ACE162}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="51.33203125" customWidth="1"/>
+    <col min="1" max="1" width="27.06640625" customWidth="1"/>
     <col min="2" max="2" width="22.796875" customWidth="1"/>
     <col min="3" max="3" width="21.6640625" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
@@ -466,10 +475,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
@@ -477,24 +489,27 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
@@ -502,15 +517,32 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
       </c>
       <c r="E5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -519,4 +551,10 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>